<commit_message>
typo in burst identifier function
</commit_message>
<xml_diff>
--- a/data/meaTable.xlsx
+++ b/data/meaTable.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianlo/Documents/GitHub/meaR/dataset1/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9881AD-74C4-FF49-A131-D31BED9887FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="7680" windowWidth="28800" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28000" windowHeight="16860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
   <si>
     <t>animalID</t>
   </si>
@@ -31,57 +27,63 @@
     <t>genotype</t>
   </si>
   <si>
+    <t>maxRecording</t>
+  </si>
+  <si>
     <t>exclude</t>
   </si>
   <si>
+    <t>channels2exclude</t>
+  </si>
+  <si>
+    <t>table comment: original</t>
+  </si>
+  <si>
+    <t>slice 1 5048.txt</t>
+  </si>
+  <si>
     <t>WT</t>
   </si>
   <si>
+    <t>slice 1 5049.txt</t>
+  </si>
+  <si>
+    <t>slice 1 5291.txt</t>
+  </si>
+  <si>
     <t>HET</t>
   </si>
   <si>
+    <t>slice 1 5295.txt</t>
+  </si>
+  <si>
+    <t>slice 1 5703.txt</t>
+  </si>
+  <si>
+    <t>slice 1 5704.txt</t>
+  </si>
+  <si>
+    <t>slice 1 5705.txt</t>
+  </si>
+  <si>
+    <t>slice 1 5707.txt</t>
+  </si>
+  <si>
+    <t>slice 1 6459.txt</t>
+  </si>
+  <si>
+    <t>slice 1 6146.txt</t>
+  </si>
+  <si>
+    <t>slice 1 6463.txt</t>
+  </si>
+  <si>
+    <t>slice 1 CL 5300.txt</t>
+  </si>
+  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>maxRecording</t>
-  </si>
-  <si>
-    <t>slice 1 5048.txt</t>
-  </si>
-  <si>
-    <t>slice 1 5049.txt</t>
-  </si>
-  <si>
-    <t>slice 1 5291.txt</t>
-  </si>
-  <si>
-    <t>slice 1 5295.txt</t>
-  </si>
-  <si>
-    <t>slice 1 5703.txt</t>
-  </si>
-  <si>
-    <t>slice 1 5704.txt</t>
-  </si>
-  <si>
-    <t>slice 1 5705.txt</t>
-  </si>
-  <si>
-    <t>slice 1 5707.txt</t>
-  </si>
-  <si>
-    <t>slice 1 6459.txt</t>
-  </si>
-  <si>
-    <t>slice 1 6146.txt</t>
-  </si>
-  <si>
-    <t>slice 1 6463.txt</t>
-  </si>
-  <si>
-    <t>slice 1 CL 5300.txt</t>
-  </si>
-  <si>
     <t>slice 2 5298.txt</t>
   </si>
   <si>
@@ -166,14 +168,35 @@
     <t>slice 3 5296.txt</t>
   </si>
   <si>
-    <t>channels2exclude</t>
+    <t>table comment: some files without bursts</t>
+  </si>
+  <si>
+    <t>slice-1-81024</t>
+  </si>
+  <si>
+    <t>slice-2-81024</t>
+  </si>
+  <si>
+    <t>slice-3-81024</t>
+  </si>
+  <si>
+    <t>slice-4-81024</t>
+  </si>
+  <si>
+    <t>table comment: reduced set from original</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,19 +208,342 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -205,9 +551,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -218,24 +806,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -493,29 +1125,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.8359375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,24 +1158,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>5048</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>1200</v>
@@ -551,7 +1186,7 @@
       <c r="F2"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>5049</v>
       </c>
@@ -559,7 +1194,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
         <v>1200</v>
@@ -567,7 +1202,7 @@
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>5291</v>
       </c>
@@ -575,548 +1210,806 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>900</v>
       </c>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>5295</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>5703</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <v>1680</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5704</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1">
         <v>1800</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>5705</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>5707</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
         <v>1200</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1">
         <v>1800</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" s="3" customFormat="1" spans="1:4">
+      <c r="A11" s="3">
         <v>6146</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3">
         <v>1500</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1">
         <v>1920</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>5300</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1">
         <v>600</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>298</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D14" s="1">
         <v>720</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>5048</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1">
         <v>2820</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>5703</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1">
         <v>1200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>5704</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1">
         <v>2340</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1">
         <v>1800</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+    <row r="19" s="3" customFormat="1" spans="1:4">
+      <c r="A19" s="3">
         <v>6146</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>6147</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1">
         <v>1860</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D21" s="1">
         <v>1800</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>298</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D22" s="1">
         <v>1260</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>5048</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1">
         <v>720</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>5291</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1">
         <v>4500</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>5292</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D25" s="1">
         <v>1500</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>5293</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D26" s="1">
         <v>2400</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>5300</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D27" s="1">
         <v>960</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>5704</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D28" s="1">
         <v>900</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D29" s="1">
         <v>1800</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>6146</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D30" s="1">
         <v>2400</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>6147</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D31" s="1">
         <v>2220</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>6163</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D32" s="1">
         <v>1800</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>63</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D33" s="1">
         <v>1800</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>5290</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D34" s="1">
         <v>6300</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>5048</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1">
         <v>1200</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>5293</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D36" s="1">
         <v>1860</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>5296</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D37" s="1">
         <v>1800</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>297</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D38" s="1">
         <v>1560</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>5296</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D39" s="1">
         <v>600</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>297</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D40" s="1">
         <v>1920</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>5296</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D41" s="1">
         <v>1800</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:E41">
+  <sortState ref="A1:E41">
     <sortCondition ref="B1:B41"/>
   </sortState>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6"/>
+  <cols>
+    <col min="1" max="1" width="8.3125" customWidth="1"/>
+    <col min="2" max="2" width="13.9375" customWidth="1"/>
+    <col min="3" max="3" width="8.875" customWidth="1"/>
+    <col min="4" max="4" width="13.25" customWidth="1"/>
+    <col min="5" max="5" width="7.6875" customWidth="1"/>
+    <col min="6" max="6" width="16.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>81024</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>81024</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>5048</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>81024</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>5049</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>81024</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5"/>
+  <cols>
+    <col min="1" max="1" width="8.3125" customWidth="1"/>
+    <col min="2" max="2" width="13.9375" customWidth="1"/>
+    <col min="3" max="3" width="8.875" customWidth="1"/>
+    <col min="4" max="4" width="13.25" customWidth="1"/>
+    <col min="5" max="5" width="7.6875" customWidth="1"/>
+    <col min="6" max="6" width="16.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>5048</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>5049</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>5291</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>900</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>5295</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1500</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>5703</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1680</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>